<commit_message>
Sanity Test Case - Regisration Flow is added now
</commit_message>
<xml_diff>
--- a/src/com/NFHS/xls/Forgot Password.xlsx
+++ b/src/com/NFHS/xls/Forgot Password.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="66">
   <si>
     <t>TCID</t>
   </si>
@@ -777,7 +777,7 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="13" customFormat="1" ht="71.25" customHeight="1">
@@ -1216,7 +1216,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>